<commit_message>
working version with wounds
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Code/CDSS Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC57466-772D-D841-8BCB-5D894153D3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9706A25D-039F-6D4A-9760-ED4AF17CB468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21780" yWindow="13240" windowWidth="15360" windowHeight="12080" xr2:uid="{3871FB82-2653-A147-BC79-29644B3BC0CE}"/>
+    <workbookView xWindow="29020" yWindow="2320" windowWidth="25500" windowHeight="12080" xr2:uid="{3871FB82-2653-A147-BC79-29644B3BC0CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>condition</t>
   </si>
@@ -58,14 +58,59 @@
     <t>Non-complicated Wounds</t>
   </si>
   <si>
-    <t xml:space="preserve">No antibiotics indicated. </t>
+    <t>Contaminated Wounds without Synovial Involvement</t>
+  </si>
+  <si>
+    <t>peroral</t>
+  </si>
+  <si>
+    <t>Trimethoprim / Sulfonamid</t>
+  </si>
+  <si>
+    <t>No, no Abscess</t>
+  </si>
+  <si>
+    <t>Pet</t>
+  </si>
+  <si>
+    <t>Chloramphenicol</t>
+  </si>
+  <si>
+    <t>No, older than 1 Month</t>
+  </si>
+  <si>
+    <t>Yes, Foal &lt; 1 Month</t>
+  </si>
+  <si>
+    <t>intravenous</t>
+  </si>
+  <si>
+    <t>intramuscular</t>
+  </si>
+  <si>
+    <t>Procain-Penicillin</t>
+  </si>
+  <si>
+    <t>Natrium-Penicillin</t>
+  </si>
+  <si>
+    <t>Gentamycin</t>
+  </si>
+  <si>
+    <t>Amikacin</t>
+  </si>
+  <si>
+    <t>Contaminated Wounds with Synovial Involvement</t>
+  </si>
+  <si>
+    <t>No antibiotics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +123,11 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,17 +159,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -438,15 +531,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCA6CB4-1F8C-2741-8D63-E91EE9F8BC95}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -474,13 +571,154 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A2 A4:A8">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="4">
       <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="3">
+      <formula>LEN(TRIM(A3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:A13">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>